<commit_message>
Fim correções turma C. Início computação notas
</commit_message>
<xml_diff>
--- a/Materias/2S2020/PED_CE342/Turma_A/output/CE342_A.xlsx
+++ b/Materias/2S2020/PED_CE342/Turma_A/output/CE342_A.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,6 +462,16 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>2020-11-09</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Resenha Novos Clássicos</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>Email</t>
         </is>
       </c>
@@ -482,7 +492,13 @@
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr">
+      <c r="F2" t="n">
+        <v>11.3</v>
+      </c>
+      <c r="G2" t="n">
+        <v>5</v>
+      </c>
+      <c r="H2" t="inlineStr">
         <is>
           <t>a212883@dac.unicamp.br</t>
         </is>
@@ -508,7 +524,13 @@
       <c r="E3" t="n">
         <v>0</v>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F3" t="n">
+        <v>14.78</v>
+      </c>
+      <c r="G3" t="n">
+        <v>10</v>
+      </c>
+      <c r="H3" t="inlineStr">
         <is>
           <t>a212900@dac.unicamp.br</t>
         </is>
@@ -534,7 +556,13 @@
       <c r="E4" t="n">
         <v>0</v>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F4" t="n">
+        <v>94.78</v>
+      </c>
+      <c r="G4" t="n">
+        <v>5</v>
+      </c>
+      <c r="H4" t="inlineStr">
         <is>
           <t>a231302@dac.unicamp.br</t>
         </is>
@@ -560,7 +588,11 @@
       <c r="E5" t="n">
         <v>0</v>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
         <is>
           <t>a231732@dac.unicamp.br</t>
         </is>
@@ -586,7 +618,13 @@
       <c r="E6" t="n">
         <v>0</v>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>10</v>
+      </c>
+      <c r="H6" t="inlineStr">
         <is>
           <t>a213360@dac.unicamp.br</t>
         </is>
@@ -612,7 +650,13 @@
       <c r="E7" t="n">
         <v>0</v>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="F7" t="n">
+        <v>13.04</v>
+      </c>
+      <c r="G7" t="n">
+        <v>5</v>
+      </c>
+      <c r="H7" t="inlineStr">
         <is>
           <t>b231898@dac.unicamp.br</t>
         </is>
@@ -638,7 +682,13 @@
       <c r="E8" t="n">
         <v>62.64</v>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="F8" t="n">
+        <v>31.3</v>
+      </c>
+      <c r="G8" t="n">
+        <v>10</v>
+      </c>
+      <c r="H8" t="inlineStr">
         <is>
           <t>b213731@dac.unicamp.br</t>
         </is>
@@ -664,7 +714,13 @@
       <c r="E9" t="n">
         <v>0</v>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="F9" t="n">
+        <v>12.17</v>
+      </c>
+      <c r="G9" t="n">
+        <v>7</v>
+      </c>
+      <c r="H9" t="inlineStr">
         <is>
           <t>b232395@dac.unicamp.br</t>
         </is>
@@ -690,7 +746,13 @@
       <c r="E10" t="n">
         <v>14.29</v>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="F10" t="n">
+        <v>18.26</v>
+      </c>
+      <c r="G10" t="n">
+        <v>5</v>
+      </c>
+      <c r="H10" t="inlineStr">
         <is>
           <t>c232796@dac.unicamp.br</t>
         </is>
@@ -716,7 +778,13 @@
       <c r="E11" t="n">
         <v>0</v>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="F11" t="n">
+        <v>12.17</v>
+      </c>
+      <c r="G11" t="n">
+        <v>5</v>
+      </c>
+      <c r="H11" t="inlineStr">
         <is>
           <t>d233335@dac.unicamp.br</t>
         </is>
@@ -742,7 +810,13 @@
       <c r="E12" t="n">
         <v>19.78</v>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="F12" t="n">
+        <v>95.65000000000001</v>
+      </c>
+      <c r="G12" t="n">
+        <v>10</v>
+      </c>
+      <c r="H12" t="inlineStr">
         <is>
           <t>e233747@dac.unicamp.br</t>
         </is>
@@ -764,7 +838,11 @@
       </c>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr">
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="inlineStr">
         <is>
           <t>f255207@dac.unicamp.br</t>
         </is>
@@ -790,7 +868,11 @@
       <c r="E14" t="n">
         <v>0</v>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr">
         <is>
           <t>g216459@dac.unicamp.br</t>
         </is>
@@ -816,7 +898,11 @@
       <c r="E15" t="n">
         <v>0</v>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="F15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr">
         <is>
           <t>g235951@dac.unicamp.br</t>
         </is>
@@ -842,7 +928,11 @@
       <c r="E16" t="n">
         <v>1.1</v>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr">
         <is>
           <t>g236276@dac.unicamp.br</t>
         </is>
@@ -868,7 +958,13 @@
       <c r="E17" t="n">
         <v>0</v>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="F17" t="n">
+        <v>93.04000000000001</v>
+      </c>
+      <c r="G17" t="n">
+        <v>10</v>
+      </c>
+      <c r="H17" t="inlineStr">
         <is>
           <t>i218090@dac.unicamp.br</t>
         </is>
@@ -894,7 +990,13 @@
       <c r="E18" t="n">
         <v>0</v>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="F18" t="n">
+        <v>87.83</v>
+      </c>
+      <c r="G18" t="n">
+        <v>7</v>
+      </c>
+      <c r="H18" t="inlineStr">
         <is>
           <t>i255241@dac.unicamp.br</t>
         </is>
@@ -920,7 +1022,13 @@
       <c r="E19" t="n">
         <v>0</v>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="F19" t="n">
+        <v>2.61</v>
+      </c>
+      <c r="G19" t="n">
+        <v>10</v>
+      </c>
+      <c r="H19" t="inlineStr">
         <is>
           <t>j237618@dac.unicamp.br</t>
         </is>
@@ -946,7 +1054,13 @@
       <c r="E20" t="n">
         <v>0</v>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="F20" t="n">
+        <v>89.56999999999999</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" t="inlineStr">
         <is>
           <t>j199735@dac.unicamp.br</t>
         </is>
@@ -972,7 +1086,13 @@
       <c r="E21" t="n">
         <v>8.789999999999999</v>
       </c>
-      <c r="F21" t="inlineStr">
+      <c r="F21" t="n">
+        <v>96.52</v>
+      </c>
+      <c r="G21" t="n">
+        <v>5</v>
+      </c>
+      <c r="H21" t="inlineStr">
         <is>
           <t>j218975@dac.unicamp.br</t>
         </is>
@@ -998,7 +1118,13 @@
       <c r="E22" t="n">
         <v>40.66</v>
       </c>
-      <c r="F22" t="inlineStr">
+      <c r="F22" t="n">
+        <v>19.13</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" t="inlineStr">
         <is>
           <t>j238414@dac.unicamp.br</t>
         </is>
@@ -1024,7 +1150,13 @@
       <c r="E23" t="n">
         <v>0</v>
       </c>
-      <c r="F23" t="inlineStr">
+      <c r="F23" t="n">
+        <v>15.65</v>
+      </c>
+      <c r="G23" t="n">
+        <v>5</v>
+      </c>
+      <c r="H23" t="inlineStr">
         <is>
           <t>k219613@dac.unicamp.br</t>
         </is>
@@ -1050,7 +1182,13 @@
       <c r="E24" t="n">
         <v>0</v>
       </c>
-      <c r="F24" t="inlineStr">
+      <c r="F24" t="n">
+        <v>40.87</v>
+      </c>
+      <c r="G24" t="n">
+        <v>7</v>
+      </c>
+      <c r="H24" t="inlineStr">
         <is>
           <t>l219907@dac.unicamp.br</t>
         </is>
@@ -1076,7 +1214,13 @@
       <c r="E25" t="n">
         <v>0</v>
       </c>
-      <c r="F25" t="inlineStr">
+      <c r="F25" t="n">
+        <v>81.73999999999999</v>
+      </c>
+      <c r="G25" t="n">
+        <v>7</v>
+      </c>
+      <c r="H25" t="inlineStr">
         <is>
           <t>l239052@dac.unicamp.br</t>
         </is>
@@ -1102,7 +1246,13 @@
       <c r="E26" t="n">
         <v>1.1</v>
       </c>
-      <c r="F26" t="inlineStr">
+      <c r="F26" t="n">
+        <v>54.78</v>
+      </c>
+      <c r="G26" t="n">
+        <v>5</v>
+      </c>
+      <c r="H26" t="inlineStr">
         <is>
           <t>l220194@dac.unicamp.br</t>
         </is>
@@ -1128,7 +1278,13 @@
       <c r="E27" t="n">
         <v>0</v>
       </c>
-      <c r="F27" t="inlineStr">
+      <c r="F27" t="n">
+        <v>6.09</v>
+      </c>
+      <c r="G27" t="n">
+        <v>10</v>
+      </c>
+      <c r="H27" t="inlineStr">
         <is>
           <t>l201326@dac.unicamp.br</t>
         </is>
@@ -1150,7 +1306,13 @@
       </c>
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr"/>
-      <c r="F28" t="inlineStr">
+      <c r="F28" t="n">
+        <v>56.52</v>
+      </c>
+      <c r="G28" t="n">
+        <v>5</v>
+      </c>
+      <c r="H28" t="inlineStr">
         <is>
           <t>l156242@dac.unicamp.br</t>
         </is>
@@ -1174,7 +1336,13 @@
       <c r="E29" t="n">
         <v>30.77</v>
       </c>
-      <c r="F29" t="inlineStr">
+      <c r="F29" t="n">
+        <v>7.83</v>
+      </c>
+      <c r="G29" t="n">
+        <v>5</v>
+      </c>
+      <c r="H29" t="inlineStr">
         <is>
           <t>l240317@dac.unicamp.br</t>
         </is>
@@ -1200,7 +1368,13 @@
       <c r="E30" t="n">
         <v>0</v>
       </c>
-      <c r="F30" t="inlineStr">
+      <c r="F30" t="n">
+        <v>8.699999999999999</v>
+      </c>
+      <c r="G30" t="n">
+        <v>7</v>
+      </c>
+      <c r="H30" t="inlineStr">
         <is>
           <t>l240409@dac.unicamp.br</t>
         </is>
@@ -1226,7 +1400,13 @@
       <c r="E31" t="n">
         <v>1.1</v>
       </c>
-      <c r="F31" t="inlineStr">
+      <c r="F31" t="n">
+        <v>42.61</v>
+      </c>
+      <c r="G31" t="n">
+        <v>5</v>
+      </c>
+      <c r="H31" t="inlineStr">
         <is>
           <t>m221515@dac.unicamp.br</t>
         </is>
@@ -1248,7 +1428,13 @@
       </c>
       <c r="D32" t="inlineStr"/>
       <c r="E32" t="inlineStr"/>
-      <c r="F32" t="inlineStr">
+      <c r="F32" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" t="inlineStr">
         <is>
           <t>m255293@dac.unicamp.br</t>
         </is>
@@ -1274,7 +1460,13 @@
       <c r="E33" t="n">
         <v>74.73</v>
       </c>
-      <c r="F33" t="inlineStr">
+      <c r="F33" t="n">
+        <v>27.83</v>
+      </c>
+      <c r="G33" t="n">
+        <v>5</v>
+      </c>
+      <c r="H33" t="inlineStr">
         <is>
           <t>m241430@dac.unicamp.br</t>
         </is>
@@ -1300,7 +1492,13 @@
       <c r="E34" t="n">
         <v>0</v>
       </c>
-      <c r="F34" t="inlineStr">
+      <c r="F34" t="n">
+        <v>7.83</v>
+      </c>
+      <c r="G34" t="n">
+        <v>10</v>
+      </c>
+      <c r="H34" t="inlineStr">
         <is>
           <t>m222315@dac.unicamp.br</t>
         </is>
@@ -1326,7 +1524,13 @@
       <c r="E35" t="n">
         <v>71.43000000000001</v>
       </c>
-      <c r="F35" t="inlineStr">
+      <c r="F35" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" t="inlineStr">
         <is>
           <t>m184528@dac.unicamp.br</t>
         </is>
@@ -1352,7 +1556,13 @@
       <c r="E36" t="n">
         <v>0</v>
       </c>
-      <c r="F36" t="inlineStr">
+      <c r="F36" t="n">
+        <v>89.56999999999999</v>
+      </c>
+      <c r="G36" t="n">
+        <v>3</v>
+      </c>
+      <c r="H36" t="inlineStr">
         <is>
           <t>m222615@dac.unicamp.br</t>
         </is>
@@ -1374,7 +1584,11 @@
       </c>
       <c r="D37" t="inlineStr"/>
       <c r="E37" t="inlineStr"/>
-      <c r="F37" t="inlineStr">
+      <c r="F37" t="inlineStr"/>
+      <c r="G37" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" t="inlineStr">
         <is>
           <t>s186966@dac.unicamp.br</t>
         </is>
@@ -1400,7 +1614,13 @@
       <c r="E38" t="n">
         <v>0</v>
       </c>
-      <c r="F38" t="inlineStr">
+      <c r="F38" t="n">
+        <v>92.17</v>
+      </c>
+      <c r="G38" t="n">
+        <v>5</v>
+      </c>
+      <c r="H38" t="inlineStr">
         <is>
           <t>s244321@dac.unicamp.br</t>
         </is>
@@ -1426,7 +1646,13 @@
       <c r="E39" t="n">
         <v>0</v>
       </c>
-      <c r="F39" t="inlineStr">
+      <c r="F39" t="n">
+        <v>79.13</v>
+      </c>
+      <c r="G39" t="n">
+        <v>5</v>
+      </c>
+      <c r="H39" t="inlineStr">
         <is>
           <t>s244379@dac.unicamp.br</t>
         </is>
@@ -1452,7 +1678,13 @@
       <c r="E40" t="n">
         <v>0</v>
       </c>
-      <c r="F40" t="inlineStr">
+      <c r="F40" t="n">
+        <v>7.83</v>
+      </c>
+      <c r="G40" t="n">
+        <v>7</v>
+      </c>
+      <c r="H40" t="inlineStr">
         <is>
           <t>t187323@dac.unicamp.br</t>
         </is>
@@ -1478,7 +1710,13 @@
       <c r="E41" t="n">
         <v>1.1</v>
       </c>
-      <c r="F41" t="inlineStr">
+      <c r="F41" t="n">
+        <v>93.91</v>
+      </c>
+      <c r="G41" t="n">
+        <v>5</v>
+      </c>
+      <c r="H41" t="inlineStr">
         <is>
           <t>t206194@dac.unicamp.br</t>
         </is>
@@ -1500,7 +1738,11 @@
       </c>
       <c r="D42" t="inlineStr"/>
       <c r="E42" t="inlineStr"/>
-      <c r="F42" t="inlineStr">
+      <c r="F42" t="inlineStr"/>
+      <c r="G42" t="n">
+        <v>10</v>
+      </c>
+      <c r="H42" t="inlineStr">
         <is>
           <t>v245212@dac.unicamp.br</t>
         </is>
@@ -1526,7 +1768,13 @@
       <c r="E43" t="n">
         <v>0</v>
       </c>
-      <c r="F43" t="inlineStr">
+      <c r="F43" t="n">
+        <v>99.13</v>
+      </c>
+      <c r="G43" t="n">
+        <v>3</v>
+      </c>
+      <c r="H43" t="inlineStr">
         <is>
           <t>v206883@dac.unicamp.br</t>
         </is>
@@ -1552,7 +1800,13 @@
       <c r="E44" t="n">
         <v>1.1</v>
       </c>
-      <c r="F44" t="inlineStr">
+      <c r="F44" t="n">
+        <v>13.91</v>
+      </c>
+      <c r="G44" t="n">
+        <v>5</v>
+      </c>
+      <c r="H44" t="inlineStr">
         <is>
           <t>v245459@dac.unicamp.br</t>
         </is>

</xml_diff>

<commit_message>
Início correções seção empírica. Restam os dois trechos sublinhados.
</commit_message>
<xml_diff>
--- a/Materias/2S2020/PED_CE342/Turma_A/output/CE342_A.xlsx
+++ b/Materias/2S2020/PED_CE342/Turma_A/output/CE342_A.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -435,153 +435,162 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>RA</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Nome</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Resenha Monetaristas</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2020-10-19</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2020-10-26</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2020-11-09</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Resenha Novos Clássicos</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Email</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>212883</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>ana pasti villalba</t>
         </is>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>50</v>
       </c>
-      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
-      <c r="F2" t="n">
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="n">
         <v>11.3</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>5</v>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>a212883@dac.unicamp.br</t>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>a0@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>212900</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>ana paula martins</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>50</v>
       </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
         <v>14.78</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>10</v>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>a212900@dac.unicamp.br</t>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>a1@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>231302</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>andré apolinário cardoso</t>
         </is>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>70</v>
       </c>
-      <c r="D4" t="n">
-        <v>0</v>
-      </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
         <v>94.78</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>5</v>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>a231302@dac.unicamp.br</t>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>a2@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>231732</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>artur preciozo figliolino</t>
         </is>
       </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
@@ -591,277 +600,304 @@
       <c r="F5" t="n">
         <v>0</v>
       </c>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>a231732@dac.unicamp.br</t>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>a3@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>213360</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>augusto lima alves</t>
         </is>
       </c>
-      <c r="C6" t="n">
+      <c r="D6" t="n">
         <v>70</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>54.03</v>
       </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
       <c r="F6" t="n">
         <v>0</v>
       </c>
       <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
         <v>10</v>
       </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>a213360@dac.unicamp.br</t>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>a4@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>231898</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>beatriz consolmagno de marchi</t>
         </is>
       </c>
-      <c r="C7" t="n">
+      <c r="D7" t="n">
         <v>70</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>1.61</v>
       </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
       <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
         <v>13.04</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>5</v>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>b231898@dac.unicamp.br</t>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>b5@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="inlineStr">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>213731</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>bianca senne roma</t>
         </is>
       </c>
-      <c r="C8" t="n">
+      <c r="D8" t="n">
         <v>70</v>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
         <v>29.03</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>62.64</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>31.3</v>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>10</v>
       </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>b213731@dac.unicamp.br</t>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>b6@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="inlineStr">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
         <is>
           <t>232395</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>bruno bueno de lima</t>
         </is>
       </c>
-      <c r="C9" t="n">
+      <c r="D9" t="n">
         <v>30</v>
       </c>
-      <c r="D9" t="n">
-        <v>0</v>
-      </c>
       <c r="E9" t="n">
         <v>0</v>
       </c>
       <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
         <v>12.17</v>
       </c>
-      <c r="G9" t="n">
+      <c r="H9" t="n">
         <v>7</v>
       </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>b232395@dac.unicamp.br</t>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>b7@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="inlineStr">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
         <is>
           <t>232796</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>carlos henrique araujo viana</t>
         </is>
       </c>
-      <c r="C10" t="n">
+      <c r="D10" t="n">
         <v>70</v>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
         <v>4.84</v>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>14.29</v>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
         <v>18.26</v>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="n">
         <v>5</v>
       </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>c232796@dac.unicamp.br</t>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>c8@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="inlineStr">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
         <is>
           <t>233335</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>danielle araujo sousa</t>
         </is>
       </c>
-      <c r="C11" t="n">
+      <c r="D11" t="n">
         <v>50</v>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
         <v>1.61</v>
       </c>
-      <c r="E11" t="n">
-        <v>0</v>
-      </c>
       <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
         <v>12.17</v>
       </c>
-      <c r="G11" t="n">
+      <c r="H11" t="n">
         <v>5</v>
       </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>d233335@dac.unicamp.br</t>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>d9@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
         <is>
           <t>233747</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>eduardo ranieri guedes pinto</t>
         </is>
       </c>
-      <c r="C12" t="n">
+      <c r="D12" t="n">
         <v>70</v>
       </c>
-      <c r="D12" t="n">
+      <c r="E12" t="n">
         <v>49.19</v>
       </c>
-      <c r="E12" t="n">
+      <c r="F12" t="n">
         <v>19.78</v>
       </c>
-      <c r="F12" t="n">
+      <c r="G12" t="n">
         <v>95.65000000000001</v>
       </c>
-      <c r="G12" t="n">
+      <c r="H12" t="n">
         <v>10</v>
       </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>e233747@dac.unicamp.br</t>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>e10@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="inlineStr">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
         <is>
           <t>255207</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>fernanda lima santos</t>
         </is>
       </c>
-      <c r="C13" t="n">
+      <c r="D13" t="n">
         <v>50</v>
       </c>
-      <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
-      <c r="G13" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>f255207@dac.unicamp.br</t>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>f11@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="inlineStr">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
         <is>
           <t>216459</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>gabriel santana rosmaninho</t>
         </is>
       </c>
-      <c r="C14" t="n">
-        <v>0</v>
-      </c>
       <c r="D14" t="n">
         <v>0</v>
       </c>
@@ -871,946 +907,1073 @@
       <c r="F14" t="n">
         <v>0</v>
       </c>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>g216459@dac.unicamp.br</t>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>g12@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="inlineStr">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
         <is>
           <t>235951</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>guilherme garcia gobbo</t>
         </is>
       </c>
-      <c r="C15" t="n">
+      <c r="D15" t="n">
         <v>30</v>
       </c>
-      <c r="D15" t="n">
+      <c r="E15" t="n">
         <v>2.42</v>
       </c>
-      <c r="E15" t="n">
-        <v>0</v>
-      </c>
       <c r="F15" t="n">
         <v>0</v>
       </c>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>g235951@dac.unicamp.br</t>
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>g13@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="inlineStr">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
         <is>
           <t>236276</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="C16" t="inlineStr">
         <is>
           <t>gustavo henrique biondi</t>
         </is>
       </c>
-      <c r="C16" t="n">
-        <v>0</v>
-      </c>
       <c r="D16" t="n">
         <v>0</v>
       </c>
       <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
         <v>1.1</v>
       </c>
-      <c r="F16" t="n">
-        <v>0</v>
-      </c>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>g236276@dac.unicamp.br</t>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>g14@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="inlineStr">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
         <is>
           <t>218090</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="C17" t="inlineStr">
         <is>
           <t>isabela de oliveira garcia</t>
         </is>
       </c>
-      <c r="C17" t="n">
+      <c r="D17" t="n">
         <v>70</v>
       </c>
-      <c r="D17" t="n">
+      <c r="E17" t="n">
         <v>1.61</v>
       </c>
-      <c r="E17" t="n">
-        <v>0</v>
-      </c>
       <c r="F17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" t="n">
         <v>93.04000000000001</v>
       </c>
-      <c r="G17" t="n">
+      <c r="H17" t="n">
         <v>10</v>
       </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>i218090@dac.unicamp.br</t>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>i15@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="inlineStr">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
         <is>
           <t>255241</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="C18" t="inlineStr">
         <is>
           <t>isabella rodrigues soares</t>
         </is>
       </c>
-      <c r="C18" t="n">
+      <c r="D18" t="n">
         <v>50</v>
       </c>
-      <c r="D18" t="n">
+      <c r="E18" t="n">
         <v>0.8100000000000001</v>
       </c>
-      <c r="E18" t="n">
-        <v>0</v>
-      </c>
       <c r="F18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" t="n">
         <v>87.83</v>
       </c>
-      <c r="G18" t="n">
+      <c r="H18" t="n">
         <v>7</v>
       </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>i255241@dac.unicamp.br</t>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>i16@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="inlineStr">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
         <is>
           <t>237618</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="C19" t="inlineStr">
         <is>
           <t>joão pedro de paula e silva</t>
         </is>
       </c>
-      <c r="C19" t="n">
+      <c r="D19" t="n">
         <v>70</v>
       </c>
-      <c r="D19" t="n">
+      <c r="E19" t="n">
         <v>2.42</v>
       </c>
-      <c r="E19" t="n">
-        <v>0</v>
-      </c>
       <c r="F19" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" t="n">
         <v>2.61</v>
       </c>
-      <c r="G19" t="n">
+      <c r="H19" t="n">
         <v>10</v>
       </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>j237618@dac.unicamp.br</t>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>j17@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="inlineStr">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
         <is>
           <t>199735</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="C20" t="inlineStr">
         <is>
           <t>joao pedro gabriel</t>
         </is>
       </c>
-      <c r="C20" t="n">
+      <c r="D20" t="n">
         <v>50</v>
       </c>
-      <c r="D20" t="n">
+      <c r="E20" t="n">
         <v>11.29</v>
       </c>
-      <c r="E20" t="n">
-        <v>0</v>
-      </c>
       <c r="F20" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" t="n">
         <v>89.56999999999999</v>
       </c>
-      <c r="G20" t="n">
-        <v>0</v>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>j199735@dac.unicamp.br</t>
+      <c r="H20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>j18@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="inlineStr">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
         <is>
           <t>218975</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="C21" t="inlineStr">
         <is>
           <t>joão vitor santos melo</t>
         </is>
       </c>
-      <c r="C21" t="n">
+      <c r="D21" t="n">
         <v>70</v>
       </c>
-      <c r="D21" t="n">
+      <c r="E21" t="n">
         <v>22.58</v>
       </c>
-      <c r="E21" t="n">
+      <c r="F21" t="n">
         <v>8.789999999999999</v>
       </c>
-      <c r="F21" t="n">
+      <c r="G21" t="n">
         <v>96.52</v>
       </c>
-      <c r="G21" t="n">
+      <c r="H21" t="n">
         <v>5</v>
       </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>j218975@dac.unicamp.br</t>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>j19@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="inlineStr">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
         <is>
           <t>238414</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="C22" t="inlineStr">
         <is>
           <t>juliana florentina fernandes leão</t>
         </is>
       </c>
-      <c r="C22" t="n">
+      <c r="D22" t="n">
         <v>70</v>
       </c>
-      <c r="D22" t="n">
+      <c r="E22" t="n">
         <v>16.94</v>
       </c>
-      <c r="E22" t="n">
+      <c r="F22" t="n">
         <v>40.66</v>
       </c>
-      <c r="F22" t="n">
+      <c r="G22" t="n">
         <v>19.13</v>
       </c>
-      <c r="G22" t="n">
-        <v>0</v>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>j238414@dac.unicamp.br</t>
+      <c r="H22" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>j20@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="inlineStr">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
         <is>
           <t>219613</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="C23" t="inlineStr">
         <is>
           <t>keivan de castro almeida g. de souza</t>
         </is>
       </c>
-      <c r="C23" t="n">
+      <c r="D23" t="n">
         <v>50</v>
       </c>
-      <c r="D23" t="n">
+      <c r="E23" t="n">
         <v>6.45</v>
       </c>
-      <c r="E23" t="n">
-        <v>0</v>
-      </c>
       <c r="F23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" t="n">
         <v>15.65</v>
       </c>
-      <c r="G23" t="n">
+      <c r="H23" t="n">
         <v>5</v>
       </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>k219613@dac.unicamp.br</t>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>k21@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="inlineStr">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
         <is>
           <t>219907</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="C24" t="inlineStr">
         <is>
           <t>laura maria alves de mattos</t>
         </is>
       </c>
-      <c r="C24" t="n">
+      <c r="D24" t="n">
         <v>100</v>
       </c>
-      <c r="D24" t="n">
+      <c r="E24" t="n">
         <v>2.42</v>
       </c>
-      <c r="E24" t="n">
-        <v>0</v>
-      </c>
       <c r="F24" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" t="n">
         <v>40.87</v>
       </c>
-      <c r="G24" t="n">
+      <c r="H24" t="n">
         <v>7</v>
       </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>l219907@dac.unicamp.br</t>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>l22@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="inlineStr">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
         <is>
           <t>239052</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="C25" t="inlineStr">
         <is>
           <t>lavínia dias de oliveira roman</t>
         </is>
       </c>
-      <c r="C25" t="n">
+      <c r="D25" t="n">
         <v>70</v>
       </c>
-      <c r="D25" t="n">
+      <c r="E25" t="n">
         <v>11.29</v>
       </c>
-      <c r="E25" t="n">
-        <v>0</v>
-      </c>
       <c r="F25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" t="n">
         <v>81.73999999999999</v>
       </c>
-      <c r="G25" t="n">
+      <c r="H25" t="n">
         <v>7</v>
       </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>l239052@dac.unicamp.br</t>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>l23@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="1" t="inlineStr">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
         <is>
           <t>220194</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
+      <c r="C26" t="inlineStr">
         <is>
           <t>leonardo tredici de souza</t>
         </is>
       </c>
-      <c r="C26" t="n">
+      <c r="D26" t="n">
         <v>70</v>
       </c>
-      <c r="D26" t="n">
+      <c r="E26" t="n">
         <v>0.8100000000000001</v>
       </c>
-      <c r="E26" t="n">
+      <c r="F26" t="n">
         <v>1.1</v>
       </c>
-      <c r="F26" t="n">
+      <c r="G26" t="n">
         <v>54.78</v>
       </c>
-      <c r="G26" t="n">
+      <c r="H26" t="n">
         <v>5</v>
       </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>l220194@dac.unicamp.br</t>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>l24@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="1" t="inlineStr">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
         <is>
           <t>201326</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
+      <c r="C27" t="inlineStr">
         <is>
           <t>leonardo vitor da silva</t>
         </is>
       </c>
-      <c r="C27" t="n">
+      <c r="D27" t="n">
         <v>50</v>
       </c>
-      <c r="D27" t="n">
+      <c r="E27" t="n">
         <v>75.81</v>
       </c>
-      <c r="E27" t="n">
-        <v>0</v>
-      </c>
       <c r="F27" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" t="n">
         <v>6.09</v>
       </c>
-      <c r="G27" t="n">
+      <c r="H27" t="n">
         <v>10</v>
       </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>l201326@dac.unicamp.br</t>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>l25@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="1" t="inlineStr">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
         <is>
           <t>156242</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="C28" t="inlineStr">
         <is>
           <t>leticia da silva cruz</t>
         </is>
       </c>
-      <c r="C28" t="n">
-        <v>0</v>
-      </c>
-      <c r="D28" t="inlineStr"/>
+      <c r="D28" t="n">
+        <v>0</v>
+      </c>
       <c r="E28" t="inlineStr"/>
-      <c r="F28" t="n">
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="n">
         <v>56.52</v>
       </c>
-      <c r="G28" t="n">
+      <c r="H28" t="n">
         <v>5</v>
       </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>l156242@dac.unicamp.br</t>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>l26@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="1" t="inlineStr">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
         <is>
           <t>240317</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="C29" t="inlineStr">
         <is>
           <t>luis felipe avi</t>
         </is>
       </c>
-      <c r="C29" t="n">
+      <c r="D29" t="n">
         <v>30</v>
       </c>
-      <c r="D29" t="inlineStr"/>
-      <c r="E29" t="n">
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="n">
         <v>30.77</v>
       </c>
-      <c r="F29" t="n">
+      <c r="G29" t="n">
         <v>7.83</v>
       </c>
-      <c r="G29" t="n">
+      <c r="H29" t="n">
         <v>5</v>
       </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>l240317@dac.unicamp.br</t>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>l27@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="1" t="inlineStr">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
         <is>
           <t>240409</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
+      <c r="C30" t="inlineStr">
         <is>
           <t>luísa mendes amstalden</t>
         </is>
       </c>
-      <c r="C30" t="n">
+      <c r="D30" t="n">
         <v>70</v>
       </c>
-      <c r="D30" t="n">
+      <c r="E30" t="n">
         <v>5.65</v>
       </c>
-      <c r="E30" t="n">
-        <v>0</v>
-      </c>
       <c r="F30" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" t="n">
         <v>8.699999999999999</v>
       </c>
-      <c r="G30" t="n">
+      <c r="H30" t="n">
         <v>7</v>
       </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>l240409@dac.unicamp.br</t>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>l28@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="inlineStr">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
         <is>
           <t>221515</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
+      <c r="C31" t="inlineStr">
         <is>
           <t>marcos baldez lagoeiro barroso</t>
         </is>
       </c>
-      <c r="C31" t="n">
+      <c r="D31" t="n">
         <v>50</v>
       </c>
-      <c r="D31" t="n">
+      <c r="E31" t="n">
         <v>0.8100000000000001</v>
       </c>
-      <c r="E31" t="n">
+      <c r="F31" t="n">
         <v>1.1</v>
       </c>
-      <c r="F31" t="n">
+      <c r="G31" t="n">
         <v>42.61</v>
       </c>
-      <c r="G31" t="n">
+      <c r="H31" t="n">
         <v>5</v>
       </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>m221515@dac.unicamp.br</t>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>m29@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="1" t="inlineStr">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
         <is>
           <t>255293</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
+      <c r="C32" t="inlineStr">
         <is>
           <t>maria júlia faustino da silva</t>
         </is>
       </c>
-      <c r="C32" t="n">
+      <c r="D32" t="n">
         <v>30</v>
       </c>
-      <c r="D32" t="inlineStr"/>
       <c r="E32" t="inlineStr"/>
-      <c r="F32" t="n">
-        <v>0</v>
-      </c>
+      <c r="F32" t="inlineStr"/>
       <c r="G32" t="n">
         <v>0</v>
       </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>m255293@dac.unicamp.br</t>
+      <c r="H32" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>m30@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="1" t="inlineStr">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
         <is>
           <t>241430</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
+      <c r="C33" t="inlineStr">
         <is>
           <t>marina de marco santucci</t>
         </is>
       </c>
-      <c r="C33" t="n">
+      <c r="D33" t="n">
         <v>50</v>
       </c>
-      <c r="D33" t="n">
-        <v>0</v>
-      </c>
       <c r="E33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" t="n">
         <v>74.73</v>
       </c>
-      <c r="F33" t="n">
+      <c r="G33" t="n">
         <v>27.83</v>
       </c>
-      <c r="G33" t="n">
+      <c r="H33" t="n">
         <v>5</v>
       </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>m241430@dac.unicamp.br</t>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>m31@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="1" t="inlineStr">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
         <is>
           <t>222315</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="C34" t="inlineStr">
         <is>
           <t>matheus oliveira lima</t>
         </is>
       </c>
-      <c r="C34" t="n">
+      <c r="D34" t="n">
         <v>50</v>
       </c>
-      <c r="D34" t="n">
+      <c r="E34" t="n">
         <v>0.8100000000000001</v>
       </c>
-      <c r="E34" t="n">
-        <v>0</v>
-      </c>
       <c r="F34" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" t="n">
         <v>7.83</v>
       </c>
-      <c r="G34" t="n">
+      <c r="H34" t="n">
         <v>10</v>
       </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>m222315@dac.unicamp.br</t>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>m32@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="1" t="inlineStr">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
         <is>
           <t>184528</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr">
+      <c r="C35" t="inlineStr">
         <is>
           <t>maycon jefferson teodoro bosing</t>
         </is>
       </c>
-      <c r="C35" t="n">
+      <c r="D35" t="n">
         <v>50</v>
       </c>
-      <c r="D35" t="n">
-        <v>0</v>
-      </c>
       <c r="E35" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" t="n">
         <v>71.43000000000001</v>
       </c>
-      <c r="F35" t="n">
-        <v>0</v>
-      </c>
       <c r="G35" t="n">
         <v>0</v>
       </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t>m184528@dac.unicamp.br</t>
+      <c r="H35" t="n">
+        <v>0</v>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>m33@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="1" t="inlineStr">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
         <is>
           <t>222615</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
+      <c r="C36" t="inlineStr">
         <is>
           <t>moises aparecido dos santos filho</t>
         </is>
       </c>
-      <c r="C36" t="n">
+      <c r="D36" t="n">
         <v>70</v>
       </c>
-      <c r="D36" t="n">
-        <v>0</v>
-      </c>
       <c r="E36" t="n">
         <v>0</v>
       </c>
       <c r="F36" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" t="n">
         <v>89.56999999999999</v>
       </c>
-      <c r="G36" t="n">
+      <c r="H36" t="n">
         <v>3</v>
       </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t>m222615@dac.unicamp.br</t>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>m34@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="1" t="inlineStr">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
         <is>
           <t>186966</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
+      <c r="C37" t="inlineStr">
         <is>
           <t>samuel henrique rezende bernardes</t>
         </is>
       </c>
-      <c r="C37" t="n">
-        <v>0</v>
-      </c>
-      <c r="D37" t="inlineStr"/>
+      <c r="D37" t="n">
+        <v>0</v>
+      </c>
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr"/>
-      <c r="G37" t="n">
-        <v>0</v>
-      </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t>s186966@dac.unicamp.br</t>
+      <c r="G37" t="inlineStr"/>
+      <c r="H37" t="n">
+        <v>0</v>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>s35@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="1" t="inlineStr">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
         <is>
           <t>244321</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr">
+      <c r="C38" t="inlineStr">
         <is>
           <t>sofia helena de oliveira nery</t>
         </is>
       </c>
-      <c r="C38" t="n">
+      <c r="D38" t="n">
         <v>50</v>
       </c>
-      <c r="D38" t="n">
+      <c r="E38" t="n">
         <v>3.23</v>
       </c>
-      <c r="E38" t="n">
-        <v>0</v>
-      </c>
       <c r="F38" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" t="n">
         <v>92.17</v>
       </c>
-      <c r="G38" t="n">
+      <c r="H38" t="n">
         <v>5</v>
       </c>
-      <c r="H38" t="inlineStr">
-        <is>
-          <t>s244321@dac.unicamp.br</t>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>s36@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="1" t="inlineStr">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
         <is>
           <t>244379</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr">
+      <c r="C39" t="inlineStr">
         <is>
           <t>stefanno felipe bicudo</t>
         </is>
       </c>
-      <c r="C39" t="n">
+      <c r="D39" t="n">
         <v>50</v>
       </c>
-      <c r="D39" t="n">
+      <c r="E39" t="n">
         <v>1.61</v>
       </c>
-      <c r="E39" t="n">
-        <v>0</v>
-      </c>
       <c r="F39" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" t="n">
         <v>79.13</v>
       </c>
-      <c r="G39" t="n">
+      <c r="H39" t="n">
         <v>5</v>
       </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>s244379@dac.unicamp.br</t>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>s37@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="1" t="inlineStr">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
         <is>
           <t>187323</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
+      <c r="C40" t="inlineStr">
         <is>
           <t>tatiana marchiori keller</t>
         </is>
       </c>
-      <c r="C40" t="n">
+      <c r="D40" t="n">
         <v>100</v>
       </c>
-      <c r="D40" t="n">
-        <v>0</v>
-      </c>
       <c r="E40" t="n">
         <v>0</v>
       </c>
       <c r="F40" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" t="n">
         <v>7.83</v>
       </c>
-      <c r="G40" t="n">
+      <c r="H40" t="n">
         <v>7</v>
       </c>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t>t187323@dac.unicamp.br</t>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>t38@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="1" t="inlineStr">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr">
         <is>
           <t>206194</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
+      <c r="C41" t="inlineStr">
         <is>
           <t>thiago alexandre ramos dos reis</t>
         </is>
       </c>
-      <c r="C41" t="n">
+      <c r="D41" t="n">
         <v>50</v>
       </c>
-      <c r="D41" t="n">
+      <c r="E41" t="n">
         <v>46.77</v>
       </c>
-      <c r="E41" t="n">
+      <c r="F41" t="n">
         <v>1.1</v>
       </c>
-      <c r="F41" t="n">
+      <c r="G41" t="n">
         <v>93.91</v>
       </c>
-      <c r="G41" t="n">
+      <c r="H41" t="n">
         <v>5</v>
       </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t>t206194@dac.unicamp.br</t>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>t39@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="1" t="inlineStr">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr">
         <is>
           <t>245212</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr">
+      <c r="C42" t="inlineStr">
         <is>
           <t>victoria silva torres santos</t>
         </is>
       </c>
-      <c r="C42" t="n">
+      <c r="D42" t="n">
         <v>100</v>
       </c>
-      <c r="D42" t="inlineStr"/>
       <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr"/>
-      <c r="G42" t="n">
+      <c r="G42" t="inlineStr"/>
+      <c r="H42" t="n">
         <v>10</v>
       </c>
-      <c r="H42" t="inlineStr">
-        <is>
-          <t>v245212@dac.unicamp.br</t>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>v40@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="1" t="inlineStr">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
         <is>
           <t>206883</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="C43" t="inlineStr">
         <is>
           <t>vinicius santos bering da silva</t>
         </is>
       </c>
-      <c r="C43" t="n">
-        <v>0</v>
-      </c>
       <c r="D43" t="n">
+        <v>0</v>
+      </c>
+      <c r="E43" t="n">
         <v>16.94</v>
       </c>
-      <c r="E43" t="n">
-        <v>0</v>
-      </c>
       <c r="F43" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" t="n">
         <v>99.13</v>
       </c>
-      <c r="G43" t="n">
+      <c r="H43" t="n">
         <v>3</v>
       </c>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t>v206883@dac.unicamp.br</t>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>v41@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="1" t="inlineStr">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="inlineStr">
         <is>
           <t>245459</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr">
+      <c r="C44" t="inlineStr">
         <is>
           <t>vinicius venancio</t>
         </is>
       </c>
-      <c r="C44" t="n">
+      <c r="D44" t="n">
         <v>70</v>
       </c>
-      <c r="D44" t="n">
+      <c r="E44" t="n">
         <v>4.84</v>
       </c>
-      <c r="E44" t="n">
+      <c r="F44" t="n">
         <v>1.1</v>
       </c>
-      <c r="F44" t="n">
+      <c r="G44" t="n">
         <v>13.91</v>
       </c>
-      <c r="G44" t="n">
+      <c r="H44" t="n">
         <v>5</v>
       </c>
-      <c r="H44" t="inlineStr">
-        <is>
-          <t>v245459@dac.unicamp.br</t>
-        </is>
-      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>v42@dac.unicamp.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t>245459</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr"/>
+      <c r="C45" t="inlineStr"/>
+      <c r="D45" t="inlineStr"/>
+      <c r="E45" t="inlineStr"/>
+      <c r="F45" t="inlineStr"/>
+      <c r="G45" t="inlineStr"/>
+      <c r="H45" t="n">
+        <v>0</v>
+      </c>
+      <c r="I45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t>238414</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr"/>
+      <c r="C46" t="inlineStr"/>
+      <c r="D46" t="inlineStr"/>
+      <c r="E46" t="inlineStr"/>
+      <c r="F46" t="inlineStr"/>
+      <c r="G46" t="inlineStr"/>
+      <c r="H46" t="n">
+        <v>5</v>
+      </c>
+      <c r="I46" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Correções turma A e C.
</commit_message>
<xml_diff>
--- a/Materias/2S2020/PED_CE342/Turma_A/output/CE342_A.xlsx
+++ b/Materias/2S2020/PED_CE342/Turma_A/output/CE342_A.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:K44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -482,6 +482,11 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
+          <t>Resenha Novos Keynesianos</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
           <t>Email</t>
         </is>
       </c>
@@ -514,7 +519,10 @@
       <c r="I2" t="n">
         <v>16.39</v>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="J2" t="n">
+        <v>5</v>
+      </c>
+      <c r="K2" t="inlineStr">
         <is>
           <t>a212883@dac.unicamp.br</t>
         </is>
@@ -552,7 +560,10 @@
       <c r="I3" t="n">
         <v>81.97</v>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="J3" t="n">
+        <v>7</v>
+      </c>
+      <c r="K3" t="inlineStr">
         <is>
           <t>a212900@dac.unicamp.br</t>
         </is>
@@ -590,7 +601,10 @@
       <c r="I4" t="n">
         <v>52.46</v>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="inlineStr">
         <is>
           <t>a231302@dac.unicamp.br</t>
         </is>
@@ -622,7 +636,8 @@
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr">
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr">
         <is>
           <t>a231732@dac.unicamp.br</t>
         </is>
@@ -660,7 +675,10 @@
       <c r="I6" t="n">
         <v>48.36</v>
       </c>
-      <c r="J6" t="inlineStr">
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="inlineStr">
         <is>
           <t>a213360@dac.unicamp.br</t>
         </is>
@@ -698,7 +716,10 @@
       <c r="I7" t="n">
         <v>54.92</v>
       </c>
-      <c r="J7" t="inlineStr">
+      <c r="J7" t="n">
+        <v>7</v>
+      </c>
+      <c r="K7" t="inlineStr">
         <is>
           <t>b231898@dac.unicamp.br</t>
         </is>
@@ -736,7 +757,10 @@
       <c r="I8" t="n">
         <v>88.52</v>
       </c>
-      <c r="J8" t="inlineStr">
+      <c r="J8" t="n">
+        <v>7</v>
+      </c>
+      <c r="K8" t="inlineStr">
         <is>
           <t>b213731@dac.unicamp.br</t>
         </is>
@@ -772,7 +796,10 @@
       <c r="I9" t="n">
         <v>3.28</v>
       </c>
-      <c r="J9" t="inlineStr">
+      <c r="J9" t="n">
+        <v>7</v>
+      </c>
+      <c r="K9" t="inlineStr">
         <is>
           <t>b232395@dac.unicamp.br</t>
         </is>
@@ -810,7 +837,10 @@
       <c r="I10" t="n">
         <v>82.79000000000001</v>
       </c>
-      <c r="J10" t="inlineStr">
+      <c r="J10" t="n">
+        <v>7</v>
+      </c>
+      <c r="K10" t="inlineStr">
         <is>
           <t>c232796@dac.unicamp.br</t>
         </is>
@@ -848,7 +878,10 @@
       <c r="I11" t="n">
         <v>18.03</v>
       </c>
-      <c r="J11" t="inlineStr">
+      <c r="J11" t="n">
+        <v>5</v>
+      </c>
+      <c r="K11" t="inlineStr">
         <is>
           <t>d233335@dac.unicamp.br</t>
         </is>
@@ -886,7 +919,10 @@
       <c r="I12" t="n">
         <v>5.74</v>
       </c>
-      <c r="J12" t="inlineStr">
+      <c r="J12" t="n">
+        <v>7</v>
+      </c>
+      <c r="K12" t="inlineStr">
         <is>
           <t>e233747@dac.unicamp.br</t>
         </is>
@@ -914,7 +950,10 @@
       </c>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr">
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="inlineStr">
         <is>
           <t>f255207@dac.unicamp.br</t>
         </is>
@@ -946,7 +985,8 @@
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr">
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr">
         <is>
           <t>g216459@dac.unicamp.br</t>
         </is>
@@ -978,7 +1018,8 @@
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr">
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr">
         <is>
           <t>g235951@dac.unicamp.br</t>
         </is>
@@ -1010,7 +1051,8 @@
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr">
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr">
         <is>
           <t>g236276@dac.unicamp.br</t>
         </is>
@@ -1048,7 +1090,10 @@
       <c r="I17" t="n">
         <v>13.11</v>
       </c>
-      <c r="J17" t="inlineStr">
+      <c r="J17" t="n">
+        <v>10</v>
+      </c>
+      <c r="K17" t="inlineStr">
         <is>
           <t>i218090@dac.unicamp.br</t>
         </is>
@@ -1086,7 +1131,10 @@
       <c r="I18" t="n">
         <v>59.02</v>
       </c>
-      <c r="J18" t="inlineStr">
+      <c r="J18" t="n">
+        <v>3</v>
+      </c>
+      <c r="K18" t="inlineStr">
         <is>
           <t>i255241@dac.unicamp.br</t>
         </is>
@@ -1124,7 +1172,10 @@
       <c r="I19" t="n">
         <v>58.2</v>
       </c>
-      <c r="J19" t="inlineStr">
+      <c r="J19" t="n">
+        <v>10</v>
+      </c>
+      <c r="K19" t="inlineStr">
         <is>
           <t>j237618@dac.unicamp.br</t>
         </is>
@@ -1162,7 +1213,10 @@
       <c r="I20" t="n">
         <v>1.64</v>
       </c>
-      <c r="J20" t="inlineStr">
+      <c r="J20" t="n">
+        <v>5</v>
+      </c>
+      <c r="K20" t="inlineStr">
         <is>
           <t>j199735@dac.unicamp.br</t>
         </is>
@@ -1200,7 +1254,10 @@
       <c r="I21" t="n">
         <v>86.89</v>
       </c>
-      <c r="J21" t="inlineStr">
+      <c r="J21" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" t="inlineStr">
         <is>
           <t>j218975@dac.unicamp.br</t>
         </is>
@@ -1238,7 +1295,10 @@
       <c r="I22" t="n">
         <v>8.199999999999999</v>
       </c>
-      <c r="J22" t="inlineStr">
+      <c r="J22" t="n">
+        <v>7</v>
+      </c>
+      <c r="K22" t="inlineStr">
         <is>
           <t>j238414@dac.unicamp.br</t>
         </is>
@@ -1272,7 +1332,10 @@
       </c>
       <c r="H23" t="inlineStr"/>
       <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr">
+      <c r="J23" t="n">
+        <v>5</v>
+      </c>
+      <c r="K23" t="inlineStr">
         <is>
           <t>k219613@dac.unicamp.br</t>
         </is>
@@ -1306,7 +1369,10 @@
       </c>
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr">
+      <c r="J24" t="n">
+        <v>10</v>
+      </c>
+      <c r="K24" t="inlineStr">
         <is>
           <t>l219907@dac.unicamp.br</t>
         </is>
@@ -1344,7 +1410,10 @@
       <c r="I25" t="n">
         <v>65.56999999999999</v>
       </c>
-      <c r="J25" t="inlineStr">
+      <c r="J25" t="n">
+        <v>7</v>
+      </c>
+      <c r="K25" t="inlineStr">
         <is>
           <t>l239052@dac.unicamp.br</t>
         </is>
@@ -1382,7 +1451,10 @@
       <c r="I26" t="n">
         <v>0</v>
       </c>
-      <c r="J26" t="inlineStr">
+      <c r="J26" t="n">
+        <v>0</v>
+      </c>
+      <c r="K26" t="inlineStr">
         <is>
           <t>l220194@dac.unicamp.br</t>
         </is>
@@ -1420,7 +1492,10 @@
       <c r="I27" t="n">
         <v>4.1</v>
       </c>
-      <c r="J27" t="inlineStr">
+      <c r="J27" t="n">
+        <v>10</v>
+      </c>
+      <c r="K27" t="inlineStr">
         <is>
           <t>l201326@dac.unicamp.br</t>
         </is>
@@ -1452,7 +1527,10 @@
       <c r="I28" t="n">
         <v>38.52</v>
       </c>
-      <c r="J28" t="inlineStr">
+      <c r="J28" t="n">
+        <v>7</v>
+      </c>
+      <c r="K28" t="inlineStr">
         <is>
           <t>l156242@dac.unicamp.br</t>
         </is>
@@ -1488,7 +1566,10 @@
       <c r="I29" t="n">
         <v>9.84</v>
       </c>
-      <c r="J29" t="inlineStr">
+      <c r="J29" t="n">
+        <v>0</v>
+      </c>
+      <c r="K29" t="inlineStr">
         <is>
           <t>l240317@dac.unicamp.br</t>
         </is>
@@ -1526,7 +1607,10 @@
       <c r="I30" t="n">
         <v>4.1</v>
       </c>
-      <c r="J30" t="inlineStr">
+      <c r="J30" t="n">
+        <v>7</v>
+      </c>
+      <c r="K30" t="inlineStr">
         <is>
           <t>l240409@dac.unicamp.br</t>
         </is>
@@ -1564,7 +1648,10 @@
       <c r="I31" t="n">
         <v>9.02</v>
       </c>
-      <c r="J31" t="inlineStr">
+      <c r="J31" t="n">
+        <v>0</v>
+      </c>
+      <c r="K31" t="inlineStr">
         <is>
           <t>m221515@dac.unicamp.br</t>
         </is>
@@ -1594,7 +1681,10 @@
       </c>
       <c r="H32" t="inlineStr"/>
       <c r="I32" t="inlineStr"/>
-      <c r="J32" t="inlineStr">
+      <c r="J32" t="n">
+        <v>0</v>
+      </c>
+      <c r="K32" t="inlineStr">
         <is>
           <t>m255293@dac.unicamp.br</t>
         </is>
@@ -1628,7 +1718,10 @@
       </c>
       <c r="H33" t="inlineStr"/>
       <c r="I33" t="inlineStr"/>
-      <c r="J33" t="inlineStr">
+      <c r="J33" t="n">
+        <v>5</v>
+      </c>
+      <c r="K33" t="inlineStr">
         <is>
           <t>m241430@dac.unicamp.br</t>
         </is>
@@ -1666,7 +1759,10 @@
       <c r="I34" t="n">
         <v>43.44</v>
       </c>
-      <c r="J34" t="inlineStr">
+      <c r="J34" t="n">
+        <v>0</v>
+      </c>
+      <c r="K34" t="inlineStr">
         <is>
           <t>m222315@dac.unicamp.br</t>
         </is>
@@ -1700,7 +1796,10 @@
       </c>
       <c r="H35" t="inlineStr"/>
       <c r="I35" t="inlineStr"/>
-      <c r="J35" t="inlineStr">
+      <c r="J35" t="n">
+        <v>0</v>
+      </c>
+      <c r="K35" t="inlineStr">
         <is>
           <t>m184528@dac.unicamp.br</t>
         </is>
@@ -1738,7 +1837,10 @@
       <c r="I36" t="n">
         <v>0</v>
       </c>
-      <c r="J36" t="inlineStr">
+      <c r="J36" t="n">
+        <v>7</v>
+      </c>
+      <c r="K36" t="inlineStr">
         <is>
           <t>m222615@dac.unicamp.br</t>
         </is>
@@ -1766,7 +1868,10 @@
       </c>
       <c r="H37" t="inlineStr"/>
       <c r="I37" t="inlineStr"/>
-      <c r="J37" t="inlineStr">
+      <c r="J37" t="n">
+        <v>0</v>
+      </c>
+      <c r="K37" t="inlineStr">
         <is>
           <t>s186966@dac.unicamp.br</t>
         </is>
@@ -1804,7 +1909,10 @@
       <c r="I38" t="n">
         <v>52.46</v>
       </c>
-      <c r="J38" t="inlineStr">
+      <c r="J38" t="n">
+        <v>0</v>
+      </c>
+      <c r="K38" t="inlineStr">
         <is>
           <t>s244321@dac.unicamp.br</t>
         </is>
@@ -1842,7 +1950,10 @@
       <c r="I39" t="n">
         <v>54.1</v>
       </c>
-      <c r="J39" t="inlineStr">
+      <c r="J39" t="n">
+        <v>0</v>
+      </c>
+      <c r="K39" t="inlineStr">
         <is>
           <t>s244379@dac.unicamp.br</t>
         </is>
@@ -1878,7 +1989,10 @@
       <c r="I40" t="n">
         <v>0.82</v>
       </c>
-      <c r="J40" t="inlineStr">
+      <c r="J40" t="n">
+        <v>0</v>
+      </c>
+      <c r="K40" t="inlineStr">
         <is>
           <t>t187323@dac.unicamp.br</t>
         </is>
@@ -1916,7 +2030,10 @@
       <c r="I41" t="n">
         <v>0</v>
       </c>
-      <c r="J41" t="inlineStr">
+      <c r="J41" t="n">
+        <v>3</v>
+      </c>
+      <c r="K41" t="inlineStr">
         <is>
           <t>t206194@dac.unicamp.br</t>
         </is>
@@ -1944,7 +2061,10 @@
       </c>
       <c r="H42" t="inlineStr"/>
       <c r="I42" t="inlineStr"/>
-      <c r="J42" t="inlineStr">
+      <c r="J42" t="n">
+        <v>0</v>
+      </c>
+      <c r="K42" t="inlineStr">
         <is>
           <t>v245212@dac.unicamp.br</t>
         </is>
@@ -1982,7 +2102,10 @@
       <c r="I43" t="n">
         <v>0.82</v>
       </c>
-      <c r="J43" t="inlineStr">
+      <c r="J43" t="n">
+        <v>7</v>
+      </c>
+      <c r="K43" t="inlineStr">
         <is>
           <t>v206883@dac.unicamp.br</t>
         </is>
@@ -2020,7 +2143,10 @@
       <c r="I44" t="n">
         <v>57.38</v>
       </c>
-      <c r="J44" t="inlineStr">
+      <c r="J44" t="n">
+        <v>0</v>
+      </c>
+      <c r="K44" t="inlineStr">
         <is>
           <t>v245459@dac.unicamp.br</t>
         </is>

</xml_diff>

<commit_message>
Ajustes relatórios turmas A e C
</commit_message>
<xml_diff>
--- a/Materias/2S2020/PED_CE342/Turma_A/output/CE342_A.xlsx
+++ b/Materias/2S2020/PED_CE342/Turma_A/output/CE342_A.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K44"/>
+  <dimension ref="A1:L44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -487,6 +487,11 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
+          <t>2020-11-30</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
           <t>Email</t>
         </is>
       </c>
@@ -522,7 +527,10 @@
       <c r="J2" t="n">
         <v>5</v>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="inlineStr">
         <is>
           <t>a212883@dac.unicamp.br</t>
         </is>
@@ -563,7 +571,10 @@
       <c r="J3" t="n">
         <v>7</v>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="K3" t="n">
+        <v>77.48</v>
+      </c>
+      <c r="L3" t="inlineStr">
         <is>
           <t>a212900@dac.unicamp.br</t>
         </is>
@@ -604,7 +615,10 @@
       <c r="J4" t="n">
         <v>0</v>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="K4" t="n">
+        <v>61.26</v>
+      </c>
+      <c r="L4" t="inlineStr">
         <is>
           <t>a231302@dac.unicamp.br</t>
         </is>
@@ -637,7 +651,8 @@
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr">
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr">
         <is>
           <t>a231732@dac.unicamp.br</t>
         </is>
@@ -678,7 +693,10 @@
       <c r="J6" t="n">
         <v>0</v>
       </c>
-      <c r="K6" t="inlineStr">
+      <c r="K6" t="n">
+        <v>43.24</v>
+      </c>
+      <c r="L6" t="inlineStr">
         <is>
           <t>a213360@dac.unicamp.br</t>
         </is>
@@ -719,7 +737,10 @@
       <c r="J7" t="n">
         <v>7</v>
       </c>
-      <c r="K7" t="inlineStr">
+      <c r="K7" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="L7" t="inlineStr">
         <is>
           <t>b231898@dac.unicamp.br</t>
         </is>
@@ -760,7 +781,10 @@
       <c r="J8" t="n">
         <v>7</v>
       </c>
-      <c r="K8" t="inlineStr">
+      <c r="K8" t="n">
+        <v>68.47</v>
+      </c>
+      <c r="L8" t="inlineStr">
         <is>
           <t>b213731@dac.unicamp.br</t>
         </is>
@@ -799,7 +823,10 @@
       <c r="J9" t="n">
         <v>7</v>
       </c>
-      <c r="K9" t="inlineStr">
+      <c r="K9" t="n">
+        <v>14.41</v>
+      </c>
+      <c r="L9" t="inlineStr">
         <is>
           <t>b232395@dac.unicamp.br</t>
         </is>
@@ -840,7 +867,10 @@
       <c r="J10" t="n">
         <v>7</v>
       </c>
-      <c r="K10" t="inlineStr">
+      <c r="K10" t="n">
+        <v>10.81</v>
+      </c>
+      <c r="L10" t="inlineStr">
         <is>
           <t>c232796@dac.unicamp.br</t>
         </is>
@@ -881,7 +911,10 @@
       <c r="J11" t="n">
         <v>5</v>
       </c>
-      <c r="K11" t="inlineStr">
+      <c r="K11" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="L11" t="inlineStr">
         <is>
           <t>d233335@dac.unicamp.br</t>
         </is>
@@ -922,7 +955,10 @@
       <c r="J12" t="n">
         <v>7</v>
       </c>
-      <c r="K12" t="inlineStr">
+      <c r="K12" t="n">
+        <v>85.59</v>
+      </c>
+      <c r="L12" t="inlineStr">
         <is>
           <t>e233747@dac.unicamp.br</t>
         </is>
@@ -953,7 +989,8 @@
       <c r="J13" t="n">
         <v>0</v>
       </c>
-      <c r="K13" t="inlineStr">
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr">
         <is>
           <t>f255207@dac.unicamp.br</t>
         </is>
@@ -986,7 +1023,8 @@
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr">
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr">
         <is>
           <t>g216459@dac.unicamp.br</t>
         </is>
@@ -1019,7 +1057,8 @@
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr">
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr">
         <is>
           <t>g235951@dac.unicamp.br</t>
         </is>
@@ -1052,7 +1091,8 @@
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr"/>
-      <c r="K16" t="inlineStr">
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr">
         <is>
           <t>g236276@dac.unicamp.br</t>
         </is>
@@ -1093,7 +1133,10 @@
       <c r="J17" t="n">
         <v>10</v>
       </c>
-      <c r="K17" t="inlineStr">
+      <c r="K17" t="n">
+        <v>68.47</v>
+      </c>
+      <c r="L17" t="inlineStr">
         <is>
           <t>i218090@dac.unicamp.br</t>
         </is>
@@ -1134,7 +1177,10 @@
       <c r="J18" t="n">
         <v>3</v>
       </c>
-      <c r="K18" t="inlineStr">
+      <c r="K18" t="n">
+        <v>45.95</v>
+      </c>
+      <c r="L18" t="inlineStr">
         <is>
           <t>i255241@dac.unicamp.br</t>
         </is>
@@ -1175,7 +1221,10 @@
       <c r="J19" t="n">
         <v>10</v>
       </c>
-      <c r="K19" t="inlineStr">
+      <c r="K19" t="n">
+        <v>89.19</v>
+      </c>
+      <c r="L19" t="inlineStr">
         <is>
           <t>j237618@dac.unicamp.br</t>
         </is>
@@ -1216,7 +1265,10 @@
       <c r="J20" t="n">
         <v>5</v>
       </c>
-      <c r="K20" t="inlineStr">
+      <c r="K20" t="n">
+        <v>88.29000000000001</v>
+      </c>
+      <c r="L20" t="inlineStr">
         <is>
           <t>j199735@dac.unicamp.br</t>
         </is>
@@ -1257,7 +1309,10 @@
       <c r="J21" t="n">
         <v>0</v>
       </c>
-      <c r="K21" t="inlineStr">
+      <c r="K21" t="n">
+        <v>85.59</v>
+      </c>
+      <c r="L21" t="inlineStr">
         <is>
           <t>j218975@dac.unicamp.br</t>
         </is>
@@ -1298,7 +1353,10 @@
       <c r="J22" t="n">
         <v>7</v>
       </c>
-      <c r="K22" t="inlineStr">
+      <c r="K22" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="L22" t="inlineStr">
         <is>
           <t>j238414@dac.unicamp.br</t>
         </is>
@@ -1335,7 +1393,8 @@
       <c r="J23" t="n">
         <v>5</v>
       </c>
-      <c r="K23" t="inlineStr">
+      <c r="K23" t="inlineStr"/>
+      <c r="L23" t="inlineStr">
         <is>
           <t>k219613@dac.unicamp.br</t>
         </is>
@@ -1372,7 +1431,8 @@
       <c r="J24" t="n">
         <v>10</v>
       </c>
-      <c r="K24" t="inlineStr">
+      <c r="K24" t="inlineStr"/>
+      <c r="L24" t="inlineStr">
         <is>
           <t>l219907@dac.unicamp.br</t>
         </is>
@@ -1413,7 +1473,10 @@
       <c r="J25" t="n">
         <v>7</v>
       </c>
-      <c r="K25" t="inlineStr">
+      <c r="K25" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="L25" t="inlineStr">
         <is>
           <t>l239052@dac.unicamp.br</t>
         </is>
@@ -1454,7 +1517,10 @@
       <c r="J26" t="n">
         <v>0</v>
       </c>
-      <c r="K26" t="inlineStr">
+      <c r="K26" t="n">
+        <v>0</v>
+      </c>
+      <c r="L26" t="inlineStr">
         <is>
           <t>l220194@dac.unicamp.br</t>
         </is>
@@ -1495,7 +1561,10 @@
       <c r="J27" t="n">
         <v>10</v>
       </c>
-      <c r="K27" t="inlineStr">
+      <c r="K27" t="n">
+        <v>91.89</v>
+      </c>
+      <c r="L27" t="inlineStr">
         <is>
           <t>l201326@dac.unicamp.br</t>
         </is>
@@ -1530,7 +1599,10 @@
       <c r="J28" t="n">
         <v>7</v>
       </c>
-      <c r="K28" t="inlineStr">
+      <c r="K28" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="L28" t="inlineStr">
         <is>
           <t>l156242@dac.unicamp.br</t>
         </is>
@@ -1569,7 +1641,10 @@
       <c r="J29" t="n">
         <v>0</v>
       </c>
-      <c r="K29" t="inlineStr">
+      <c r="K29" t="n">
+        <v>8.109999999999999</v>
+      </c>
+      <c r="L29" t="inlineStr">
         <is>
           <t>l240317@dac.unicamp.br</t>
         </is>
@@ -1610,7 +1685,10 @@
       <c r="J30" t="n">
         <v>7</v>
       </c>
-      <c r="K30" t="inlineStr">
+      <c r="K30" t="n">
+        <v>0</v>
+      </c>
+      <c r="L30" t="inlineStr">
         <is>
           <t>l240409@dac.unicamp.br</t>
         </is>
@@ -1651,7 +1729,10 @@
       <c r="J31" t="n">
         <v>0</v>
       </c>
-      <c r="K31" t="inlineStr">
+      <c r="K31" t="n">
+        <v>81.98</v>
+      </c>
+      <c r="L31" t="inlineStr">
         <is>
           <t>m221515@dac.unicamp.br</t>
         </is>
@@ -1684,7 +1765,8 @@
       <c r="J32" t="n">
         <v>0</v>
       </c>
-      <c r="K32" t="inlineStr">
+      <c r="K32" t="inlineStr"/>
+      <c r="L32" t="inlineStr">
         <is>
           <t>m255293@dac.unicamp.br</t>
         </is>
@@ -1721,7 +1803,10 @@
       <c r="J33" t="n">
         <v>5</v>
       </c>
-      <c r="K33" t="inlineStr">
+      <c r="K33" t="n">
+        <v>61.26</v>
+      </c>
+      <c r="L33" t="inlineStr">
         <is>
           <t>m241430@dac.unicamp.br</t>
         </is>
@@ -1762,7 +1847,10 @@
       <c r="J34" t="n">
         <v>0</v>
       </c>
-      <c r="K34" t="inlineStr">
+      <c r="K34" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="L34" t="inlineStr">
         <is>
           <t>m222315@dac.unicamp.br</t>
         </is>
@@ -1799,7 +1887,8 @@
       <c r="J35" t="n">
         <v>0</v>
       </c>
-      <c r="K35" t="inlineStr">
+      <c r="K35" t="inlineStr"/>
+      <c r="L35" t="inlineStr">
         <is>
           <t>m184528@dac.unicamp.br</t>
         </is>
@@ -1840,7 +1929,10 @@
       <c r="J36" t="n">
         <v>7</v>
       </c>
-      <c r="K36" t="inlineStr">
+      <c r="K36" t="n">
+        <v>82.88</v>
+      </c>
+      <c r="L36" t="inlineStr">
         <is>
           <t>m222615@dac.unicamp.br</t>
         </is>
@@ -1871,7 +1963,8 @@
       <c r="J37" t="n">
         <v>0</v>
       </c>
-      <c r="K37" t="inlineStr">
+      <c r="K37" t="inlineStr"/>
+      <c r="L37" t="inlineStr">
         <is>
           <t>s186966@dac.unicamp.br</t>
         </is>
@@ -1912,7 +2005,10 @@
       <c r="J38" t="n">
         <v>0</v>
       </c>
-      <c r="K38" t="inlineStr">
+      <c r="K38" t="n">
+        <v>7.21</v>
+      </c>
+      <c r="L38" t="inlineStr">
         <is>
           <t>s244321@dac.unicamp.br</t>
         </is>
@@ -1953,7 +2049,10 @@
       <c r="J39" t="n">
         <v>0</v>
       </c>
-      <c r="K39" t="inlineStr">
+      <c r="K39" t="n">
+        <v>90.98999999999999</v>
+      </c>
+      <c r="L39" t="inlineStr">
         <is>
           <t>s244379@dac.unicamp.br</t>
         </is>
@@ -1992,7 +2091,10 @@
       <c r="J40" t="n">
         <v>0</v>
       </c>
-      <c r="K40" t="inlineStr">
+      <c r="K40" t="n">
+        <v>0</v>
+      </c>
+      <c r="L40" t="inlineStr">
         <is>
           <t>t187323@dac.unicamp.br</t>
         </is>
@@ -2033,7 +2135,10 @@
       <c r="J41" t="n">
         <v>3</v>
       </c>
-      <c r="K41" t="inlineStr">
+      <c r="K41" t="n">
+        <v>92.79000000000001</v>
+      </c>
+      <c r="L41" t="inlineStr">
         <is>
           <t>t206194@dac.unicamp.br</t>
         </is>
@@ -2064,7 +2169,8 @@
       <c r="J42" t="n">
         <v>0</v>
       </c>
-      <c r="K42" t="inlineStr">
+      <c r="K42" t="inlineStr"/>
+      <c r="L42" t="inlineStr">
         <is>
           <t>v245212@dac.unicamp.br</t>
         </is>
@@ -2105,7 +2211,10 @@
       <c r="J43" t="n">
         <v>7</v>
       </c>
-      <c r="K43" t="inlineStr">
+      <c r="K43" t="n">
+        <v>35.14</v>
+      </c>
+      <c r="L43" t="inlineStr">
         <is>
           <t>v206883@dac.unicamp.br</t>
         </is>
@@ -2146,7 +2255,10 @@
       <c r="J44" t="n">
         <v>0</v>
       </c>
-      <c r="K44" t="inlineStr">
+      <c r="K44" t="n">
+        <v>0</v>
+      </c>
+      <c r="L44" t="inlineStr">
         <is>
           <t>v245459@dac.unicamp.br</t>
         </is>

</xml_diff>

<commit_message>
Relatórios turmas A e C
</commit_message>
<xml_diff>
--- a/Materias/2S2020/PED_CE342/Turma_A/output/CE342_A.xlsx
+++ b/Materias/2S2020/PED_CE342/Turma_A/output/CE342_A.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L44"/>
+  <dimension ref="A1:M44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -492,6 +492,11 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
+          <t>Resenha Regime de Metas</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
           <t>Email</t>
         </is>
       </c>
@@ -530,7 +535,10 @@
       <c r="K2" t="n">
         <v>0</v>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="inlineStr">
         <is>
           <t>a212883@dac.unicamp.br</t>
         </is>
@@ -574,7 +582,10 @@
       <c r="K3" t="n">
         <v>77.48</v>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="L3" t="n">
+        <v>5</v>
+      </c>
+      <c r="M3" t="inlineStr">
         <is>
           <t>a212900@dac.unicamp.br</t>
         </is>
@@ -618,7 +629,10 @@
       <c r="K4" t="n">
         <v>61.26</v>
       </c>
-      <c r="L4" t="inlineStr">
+      <c r="L4" t="n">
+        <v>7</v>
+      </c>
+      <c r="M4" t="inlineStr">
         <is>
           <t>a231302@dac.unicamp.br</t>
         </is>
@@ -652,7 +666,8 @@
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr">
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr">
         <is>
           <t>a231732@dac.unicamp.br</t>
         </is>
@@ -696,7 +711,10 @@
       <c r="K6" t="n">
         <v>43.24</v>
       </c>
-      <c r="L6" t="inlineStr">
+      <c r="L6" t="n">
+        <v>10</v>
+      </c>
+      <c r="M6" t="inlineStr">
         <is>
           <t>a213360@dac.unicamp.br</t>
         </is>
@@ -740,7 +758,10 @@
       <c r="K7" t="n">
         <v>0.9</v>
       </c>
-      <c r="L7" t="inlineStr">
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="inlineStr">
         <is>
           <t>b231898@dac.unicamp.br</t>
         </is>
@@ -784,7 +805,10 @@
       <c r="K8" t="n">
         <v>68.47</v>
       </c>
-      <c r="L8" t="inlineStr">
+      <c r="L8" t="n">
+        <v>7</v>
+      </c>
+      <c r="M8" t="inlineStr">
         <is>
           <t>b213731@dac.unicamp.br</t>
         </is>
@@ -826,7 +850,10 @@
       <c r="K9" t="n">
         <v>14.41</v>
       </c>
-      <c r="L9" t="inlineStr">
+      <c r="L9" t="n">
+        <v>5</v>
+      </c>
+      <c r="M9" t="inlineStr">
         <is>
           <t>b232395@dac.unicamp.br</t>
         </is>
@@ -870,7 +897,10 @@
       <c r="K10" t="n">
         <v>10.81</v>
       </c>
-      <c r="L10" t="inlineStr">
+      <c r="L10" t="n">
+        <v>5</v>
+      </c>
+      <c r="M10" t="inlineStr">
         <is>
           <t>c232796@dac.unicamp.br</t>
         </is>
@@ -914,7 +944,10 @@
       <c r="K11" t="n">
         <v>0.9</v>
       </c>
-      <c r="L11" t="inlineStr">
+      <c r="L11" t="n">
+        <v>5</v>
+      </c>
+      <c r="M11" t="inlineStr">
         <is>
           <t>d233335@dac.unicamp.br</t>
         </is>
@@ -958,7 +991,10 @@
       <c r="K12" t="n">
         <v>85.59</v>
       </c>
-      <c r="L12" t="inlineStr">
+      <c r="L12" t="n">
+        <v>7</v>
+      </c>
+      <c r="M12" t="inlineStr">
         <is>
           <t>e233747@dac.unicamp.br</t>
         </is>
@@ -990,7 +1026,10 @@
         <v>0</v>
       </c>
       <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr">
+      <c r="L13" t="n">
+        <v>5</v>
+      </c>
+      <c r="M13" t="inlineStr">
         <is>
           <t>f255207@dac.unicamp.br</t>
         </is>
@@ -1024,7 +1063,8 @@
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
-      <c r="L14" t="inlineStr">
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr">
         <is>
           <t>g216459@dac.unicamp.br</t>
         </is>
@@ -1058,7 +1098,8 @@
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr"/>
-      <c r="L15" t="inlineStr">
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr">
         <is>
           <t>g235951@dac.unicamp.br</t>
         </is>
@@ -1092,7 +1133,8 @@
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr"/>
-      <c r="L16" t="inlineStr">
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr">
         <is>
           <t>g236276@dac.unicamp.br</t>
         </is>
@@ -1136,7 +1178,10 @@
       <c r="K17" t="n">
         <v>68.47</v>
       </c>
-      <c r="L17" t="inlineStr">
+      <c r="L17" t="n">
+        <v>10</v>
+      </c>
+      <c r="M17" t="inlineStr">
         <is>
           <t>i218090@dac.unicamp.br</t>
         </is>
@@ -1180,7 +1225,10 @@
       <c r="K18" t="n">
         <v>45.95</v>
       </c>
-      <c r="L18" t="inlineStr">
+      <c r="L18" t="n">
+        <v>5</v>
+      </c>
+      <c r="M18" t="inlineStr">
         <is>
           <t>i255241@dac.unicamp.br</t>
         </is>
@@ -1224,7 +1272,10 @@
       <c r="K19" t="n">
         <v>89.19</v>
       </c>
-      <c r="L19" t="inlineStr">
+      <c r="L19" t="n">
+        <v>10</v>
+      </c>
+      <c r="M19" t="inlineStr">
         <is>
           <t>j237618@dac.unicamp.br</t>
         </is>
@@ -1268,7 +1319,10 @@
       <c r="K20" t="n">
         <v>88.29000000000001</v>
       </c>
-      <c r="L20" t="inlineStr">
+      <c r="L20" t="n">
+        <v>0</v>
+      </c>
+      <c r="M20" t="inlineStr">
         <is>
           <t>j199735@dac.unicamp.br</t>
         </is>
@@ -1312,7 +1366,10 @@
       <c r="K21" t="n">
         <v>85.59</v>
       </c>
-      <c r="L21" t="inlineStr">
+      <c r="L21" t="n">
+        <v>7</v>
+      </c>
+      <c r="M21" t="inlineStr">
         <is>
           <t>j218975@dac.unicamp.br</t>
         </is>
@@ -1356,7 +1413,10 @@
       <c r="K22" t="n">
         <v>3.6</v>
       </c>
-      <c r="L22" t="inlineStr">
+      <c r="L22" t="n">
+        <v>10</v>
+      </c>
+      <c r="M22" t="inlineStr">
         <is>
           <t>j238414@dac.unicamp.br</t>
         </is>
@@ -1394,7 +1454,10 @@
         <v>5</v>
       </c>
       <c r="K23" t="inlineStr"/>
-      <c r="L23" t="inlineStr">
+      <c r="L23" t="n">
+        <v>0</v>
+      </c>
+      <c r="M23" t="inlineStr">
         <is>
           <t>k219613@dac.unicamp.br</t>
         </is>
@@ -1432,7 +1495,10 @@
         <v>10</v>
       </c>
       <c r="K24" t="inlineStr"/>
-      <c r="L24" t="inlineStr">
+      <c r="L24" t="n">
+        <v>0</v>
+      </c>
+      <c r="M24" t="inlineStr">
         <is>
           <t>l219907@dac.unicamp.br</t>
         </is>
@@ -1476,7 +1542,10 @@
       <c r="K25" t="n">
         <v>4.5</v>
       </c>
-      <c r="L25" t="inlineStr">
+      <c r="L25" t="n">
+        <v>0</v>
+      </c>
+      <c r="M25" t="inlineStr">
         <is>
           <t>l239052@dac.unicamp.br</t>
         </is>
@@ -1520,7 +1589,10 @@
       <c r="K26" t="n">
         <v>0</v>
       </c>
-      <c r="L26" t="inlineStr">
+      <c r="L26" t="n">
+        <v>0</v>
+      </c>
+      <c r="M26" t="inlineStr">
         <is>
           <t>l220194@dac.unicamp.br</t>
         </is>
@@ -1564,7 +1636,10 @@
       <c r="K27" t="n">
         <v>91.89</v>
       </c>
-      <c r="L27" t="inlineStr">
+      <c r="L27" t="n">
+        <v>10</v>
+      </c>
+      <c r="M27" t="inlineStr">
         <is>
           <t>l201326@dac.unicamp.br</t>
         </is>
@@ -1602,7 +1677,10 @@
       <c r="K28" t="n">
         <v>3.6</v>
       </c>
-      <c r="L28" t="inlineStr">
+      <c r="L28" t="n">
+        <v>10</v>
+      </c>
+      <c r="M28" t="inlineStr">
         <is>
           <t>l156242@dac.unicamp.br</t>
         </is>
@@ -1644,7 +1722,8 @@
       <c r="K29" t="n">
         <v>8.109999999999999</v>
       </c>
-      <c r="L29" t="inlineStr">
+      <c r="L29" t="inlineStr"/>
+      <c r="M29" t="inlineStr">
         <is>
           <t>l240317@dac.unicamp.br</t>
         </is>
@@ -1688,7 +1767,10 @@
       <c r="K30" t="n">
         <v>0</v>
       </c>
-      <c r="L30" t="inlineStr">
+      <c r="L30" t="n">
+        <v>0</v>
+      </c>
+      <c r="M30" t="inlineStr">
         <is>
           <t>l240409@dac.unicamp.br</t>
         </is>
@@ -1732,7 +1814,10 @@
       <c r="K31" t="n">
         <v>81.98</v>
       </c>
-      <c r="L31" t="inlineStr">
+      <c r="L31" t="n">
+        <v>7</v>
+      </c>
+      <c r="M31" t="inlineStr">
         <is>
           <t>m221515@dac.unicamp.br</t>
         </is>
@@ -1766,7 +1851,10 @@
         <v>0</v>
       </c>
       <c r="K32" t="inlineStr"/>
-      <c r="L32" t="inlineStr">
+      <c r="L32" t="n">
+        <v>0</v>
+      </c>
+      <c r="M32" t="inlineStr">
         <is>
           <t>m255293@dac.unicamp.br</t>
         </is>
@@ -1806,7 +1894,10 @@
       <c r="K33" t="n">
         <v>61.26</v>
       </c>
-      <c r="L33" t="inlineStr">
+      <c r="L33" t="n">
+        <v>0</v>
+      </c>
+      <c r="M33" t="inlineStr">
         <is>
           <t>m241430@dac.unicamp.br</t>
         </is>
@@ -1850,7 +1941,10 @@
       <c r="K34" t="n">
         <v>2.7</v>
       </c>
-      <c r="L34" t="inlineStr">
+      <c r="L34" t="n">
+        <v>7</v>
+      </c>
+      <c r="M34" t="inlineStr">
         <is>
           <t>m222315@dac.unicamp.br</t>
         </is>
@@ -1888,7 +1982,10 @@
         <v>0</v>
       </c>
       <c r="K35" t="inlineStr"/>
-      <c r="L35" t="inlineStr">
+      <c r="L35" t="n">
+        <v>5</v>
+      </c>
+      <c r="M35" t="inlineStr">
         <is>
           <t>m184528@dac.unicamp.br</t>
         </is>
@@ -1932,7 +2029,10 @@
       <c r="K36" t="n">
         <v>82.88</v>
       </c>
-      <c r="L36" t="inlineStr">
+      <c r="L36" t="n">
+        <v>10</v>
+      </c>
+      <c r="M36" t="inlineStr">
         <is>
           <t>m222615@dac.unicamp.br</t>
         </is>
@@ -1964,7 +2064,10 @@
         <v>0</v>
       </c>
       <c r="K37" t="inlineStr"/>
-      <c r="L37" t="inlineStr">
+      <c r="L37" t="n">
+        <v>0</v>
+      </c>
+      <c r="M37" t="inlineStr">
         <is>
           <t>s186966@dac.unicamp.br</t>
         </is>
@@ -2008,7 +2111,10 @@
       <c r="K38" t="n">
         <v>7.21</v>
       </c>
-      <c r="L38" t="inlineStr">
+      <c r="L38" t="n">
+        <v>5</v>
+      </c>
+      <c r="M38" t="inlineStr">
         <is>
           <t>s244321@dac.unicamp.br</t>
         </is>
@@ -2052,7 +2158,10 @@
       <c r="K39" t="n">
         <v>90.98999999999999</v>
       </c>
-      <c r="L39" t="inlineStr">
+      <c r="L39" t="n">
+        <v>7</v>
+      </c>
+      <c r="M39" t="inlineStr">
         <is>
           <t>s244379@dac.unicamp.br</t>
         </is>
@@ -2094,7 +2203,10 @@
       <c r="K40" t="n">
         <v>0</v>
       </c>
-      <c r="L40" t="inlineStr">
+      <c r="L40" t="n">
+        <v>10</v>
+      </c>
+      <c r="M40" t="inlineStr">
         <is>
           <t>t187323@dac.unicamp.br</t>
         </is>
@@ -2138,7 +2250,10 @@
       <c r="K41" t="n">
         <v>92.79000000000001</v>
       </c>
-      <c r="L41" t="inlineStr">
+      <c r="L41" t="n">
+        <v>0</v>
+      </c>
+      <c r="M41" t="inlineStr">
         <is>
           <t>t206194@dac.unicamp.br</t>
         </is>
@@ -2170,7 +2285,10 @@
         <v>0</v>
       </c>
       <c r="K42" t="inlineStr"/>
-      <c r="L42" t="inlineStr">
+      <c r="L42" t="n">
+        <v>10</v>
+      </c>
+      <c r="M42" t="inlineStr">
         <is>
           <t>v245212@dac.unicamp.br</t>
         </is>
@@ -2214,7 +2332,10 @@
       <c r="K43" t="n">
         <v>35.14</v>
       </c>
-      <c r="L43" t="inlineStr">
+      <c r="L43" t="n">
+        <v>7</v>
+      </c>
+      <c r="M43" t="inlineStr">
         <is>
           <t>v206883@dac.unicamp.br</t>
         </is>
@@ -2258,7 +2379,10 @@
       <c r="K44" t="n">
         <v>0</v>
       </c>
-      <c r="L44" t="inlineStr">
+      <c r="L44" t="n">
+        <v>7</v>
+      </c>
+      <c r="M44" t="inlineStr">
         <is>
           <t>v245459@dac.unicamp.br</t>
         </is>

</xml_diff>

<commit_message>
Presença turma A. Script Cecon Covid
</commit_message>
<xml_diff>
--- a/Materias/2S2020/PED_CE342/Turma_A/output/CE342_A.xlsx
+++ b/Materias/2S2020/PED_CE342/Turma_A/output/CE342_A.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M44"/>
+  <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -497,6 +497,11 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
+          <t>2020-12-14</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
           <t>Email</t>
         </is>
       </c>
@@ -538,7 +543,10 @@
       <c r="L2" t="n">
         <v>0</v>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="inlineStr">
         <is>
           <t>a212883@dac.unicamp.br</t>
         </is>
@@ -585,7 +593,10 @@
       <c r="L3" t="n">
         <v>5</v>
       </c>
-      <c r="M3" t="inlineStr">
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="inlineStr">
         <is>
           <t>a212900@dac.unicamp.br</t>
         </is>
@@ -632,7 +643,10 @@
       <c r="L4" t="n">
         <v>7</v>
       </c>
-      <c r="M4" t="inlineStr">
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="inlineStr">
         <is>
           <t>a231302@dac.unicamp.br</t>
         </is>
@@ -667,7 +681,10 @@
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr">
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="inlineStr">
         <is>
           <t>a231732@dac.unicamp.br</t>
         </is>
@@ -714,7 +731,10 @@
       <c r="L6" t="n">
         <v>10</v>
       </c>
-      <c r="M6" t="inlineStr">
+      <c r="M6" t="n">
+        <v>27.96</v>
+      </c>
+      <c r="N6" t="inlineStr">
         <is>
           <t>a213360@dac.unicamp.br</t>
         </is>
@@ -761,7 +781,10 @@
       <c r="L7" t="n">
         <v>0</v>
       </c>
-      <c r="M7" t="inlineStr">
+      <c r="M7" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="N7" t="inlineStr">
         <is>
           <t>b231898@dac.unicamp.br</t>
         </is>
@@ -808,7 +831,10 @@
       <c r="L8" t="n">
         <v>7</v>
       </c>
-      <c r="M8" t="inlineStr">
+      <c r="M8" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="N8" t="inlineStr">
         <is>
           <t>b213731@dac.unicamp.br</t>
         </is>
@@ -853,7 +879,10 @@
       <c r="L9" t="n">
         <v>5</v>
       </c>
-      <c r="M9" t="inlineStr">
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="inlineStr">
         <is>
           <t>b232395@dac.unicamp.br</t>
         </is>
@@ -900,7 +929,10 @@
       <c r="L10" t="n">
         <v>5</v>
       </c>
-      <c r="M10" t="inlineStr">
+      <c r="M10" t="n">
+        <v>70.97</v>
+      </c>
+      <c r="N10" t="inlineStr">
         <is>
           <t>c232796@dac.unicamp.br</t>
         </is>
@@ -947,7 +979,10 @@
       <c r="L11" t="n">
         <v>5</v>
       </c>
-      <c r="M11" t="inlineStr">
+      <c r="M11" t="n">
+        <v>2.15</v>
+      </c>
+      <c r="N11" t="inlineStr">
         <is>
           <t>d233335@dac.unicamp.br</t>
         </is>
@@ -994,7 +1029,10 @@
       <c r="L12" t="n">
         <v>7</v>
       </c>
-      <c r="M12" t="inlineStr">
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="inlineStr">
         <is>
           <t>e233747@dac.unicamp.br</t>
         </is>
@@ -1029,7 +1067,8 @@
       <c r="L13" t="n">
         <v>5</v>
       </c>
-      <c r="M13" t="inlineStr">
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr">
         <is>
           <t>f255207@dac.unicamp.br</t>
         </is>
@@ -1064,7 +1103,10 @@
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr">
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" t="inlineStr">
         <is>
           <t>g216459@dac.unicamp.br</t>
         </is>
@@ -1099,7 +1141,10 @@
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr"/>
-      <c r="M15" t="inlineStr">
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" t="inlineStr">
         <is>
           <t>g235951@dac.unicamp.br</t>
         </is>
@@ -1134,7 +1179,10 @@
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr"/>
-      <c r="M16" t="inlineStr">
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" t="inlineStr">
         <is>
           <t>g236276@dac.unicamp.br</t>
         </is>
@@ -1181,7 +1229,10 @@
       <c r="L17" t="n">
         <v>10</v>
       </c>
-      <c r="M17" t="inlineStr">
+      <c r="M17" t="n">
+        <v>18.28</v>
+      </c>
+      <c r="N17" t="inlineStr">
         <is>
           <t>i218090@dac.unicamp.br</t>
         </is>
@@ -1228,7 +1279,10 @@
       <c r="L18" t="n">
         <v>5</v>
       </c>
-      <c r="M18" t="inlineStr">
+      <c r="M18" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" t="inlineStr">
         <is>
           <t>i255241@dac.unicamp.br</t>
         </is>
@@ -1275,7 +1329,10 @@
       <c r="L19" t="n">
         <v>10</v>
       </c>
-      <c r="M19" t="inlineStr">
+      <c r="M19" t="n">
+        <v>0</v>
+      </c>
+      <c r="N19" t="inlineStr">
         <is>
           <t>j237618@dac.unicamp.br</t>
         </is>
@@ -1322,7 +1379,10 @@
       <c r="L20" t="n">
         <v>0</v>
       </c>
-      <c r="M20" t="inlineStr">
+      <c r="M20" t="n">
+        <v>36.56</v>
+      </c>
+      <c r="N20" t="inlineStr">
         <is>
           <t>j199735@dac.unicamp.br</t>
         </is>
@@ -1369,7 +1429,10 @@
       <c r="L21" t="n">
         <v>7</v>
       </c>
-      <c r="M21" t="inlineStr">
+      <c r="M21" t="n">
+        <v>17.2</v>
+      </c>
+      <c r="N21" t="inlineStr">
         <is>
           <t>j218975@dac.unicamp.br</t>
         </is>
@@ -1416,7 +1479,10 @@
       <c r="L22" t="n">
         <v>10</v>
       </c>
-      <c r="M22" t="inlineStr">
+      <c r="M22" t="n">
+        <v>0</v>
+      </c>
+      <c r="N22" t="inlineStr">
         <is>
           <t>j238414@dac.unicamp.br</t>
         </is>
@@ -1457,7 +1523,10 @@
       <c r="L23" t="n">
         <v>0</v>
       </c>
-      <c r="M23" t="inlineStr">
+      <c r="M23" t="n">
+        <v>0</v>
+      </c>
+      <c r="N23" t="inlineStr">
         <is>
           <t>k219613@dac.unicamp.br</t>
         </is>
@@ -1498,7 +1567,10 @@
       <c r="L24" t="n">
         <v>0</v>
       </c>
-      <c r="M24" t="inlineStr">
+      <c r="M24" t="n">
+        <v>0</v>
+      </c>
+      <c r="N24" t="inlineStr">
         <is>
           <t>l219907@dac.unicamp.br</t>
         </is>
@@ -1545,7 +1617,10 @@
       <c r="L25" t="n">
         <v>0</v>
       </c>
-      <c r="M25" t="inlineStr">
+      <c r="M25" t="n">
+        <v>0</v>
+      </c>
+      <c r="N25" t="inlineStr">
         <is>
           <t>l239052@dac.unicamp.br</t>
         </is>
@@ -1592,7 +1667,10 @@
       <c r="L26" t="n">
         <v>0</v>
       </c>
-      <c r="M26" t="inlineStr">
+      <c r="M26" t="n">
+        <v>0</v>
+      </c>
+      <c r="N26" t="inlineStr">
         <is>
           <t>l220194@dac.unicamp.br</t>
         </is>
@@ -1639,7 +1717,10 @@
       <c r="L27" t="n">
         <v>10</v>
       </c>
-      <c r="M27" t="inlineStr">
+      <c r="M27" t="n">
+        <v>3.23</v>
+      </c>
+      <c r="N27" t="inlineStr">
         <is>
           <t>l201326@dac.unicamp.br</t>
         </is>
@@ -1680,7 +1761,10 @@
       <c r="L28" t="n">
         <v>10</v>
       </c>
-      <c r="M28" t="inlineStr">
+      <c r="M28" t="n">
+        <v>0</v>
+      </c>
+      <c r="N28" t="inlineStr">
         <is>
           <t>l156242@dac.unicamp.br</t>
         </is>
@@ -1723,7 +1807,10 @@
         <v>8.109999999999999</v>
       </c>
       <c r="L29" t="inlineStr"/>
-      <c r="M29" t="inlineStr">
+      <c r="M29" t="n">
+        <v>0</v>
+      </c>
+      <c r="N29" t="inlineStr">
         <is>
           <t>l240317@dac.unicamp.br</t>
         </is>
@@ -1770,7 +1857,10 @@
       <c r="L30" t="n">
         <v>0</v>
       </c>
-      <c r="M30" t="inlineStr">
+      <c r="M30" t="n">
+        <v>0</v>
+      </c>
+      <c r="N30" t="inlineStr">
         <is>
           <t>l240409@dac.unicamp.br</t>
         </is>
@@ -1817,7 +1907,10 @@
       <c r="L31" t="n">
         <v>7</v>
       </c>
-      <c r="M31" t="inlineStr">
+      <c r="M31" t="n">
+        <v>16.13</v>
+      </c>
+      <c r="N31" t="inlineStr">
         <is>
           <t>m221515@dac.unicamp.br</t>
         </is>
@@ -1854,7 +1947,10 @@
       <c r="L32" t="n">
         <v>0</v>
       </c>
-      <c r="M32" t="inlineStr">
+      <c r="M32" t="n">
+        <v>0</v>
+      </c>
+      <c r="N32" t="inlineStr">
         <is>
           <t>m255293@dac.unicamp.br</t>
         </is>
@@ -1897,7 +1993,10 @@
       <c r="L33" t="n">
         <v>0</v>
       </c>
-      <c r="M33" t="inlineStr">
+      <c r="M33" t="n">
+        <v>0</v>
+      </c>
+      <c r="N33" t="inlineStr">
         <is>
           <t>m241430@dac.unicamp.br</t>
         </is>
@@ -1944,7 +2043,10 @@
       <c r="L34" t="n">
         <v>7</v>
       </c>
-      <c r="M34" t="inlineStr">
+      <c r="M34" t="n">
+        <v>0</v>
+      </c>
+      <c r="N34" t="inlineStr">
         <is>
           <t>m222315@dac.unicamp.br</t>
         </is>
@@ -1985,7 +2087,10 @@
       <c r="L35" t="n">
         <v>5</v>
       </c>
-      <c r="M35" t="inlineStr">
+      <c r="M35" t="n">
+        <v>0</v>
+      </c>
+      <c r="N35" t="inlineStr">
         <is>
           <t>m184528@dac.unicamp.br</t>
         </is>
@@ -2032,7 +2137,10 @@
       <c r="L36" t="n">
         <v>10</v>
       </c>
-      <c r="M36" t="inlineStr">
+      <c r="M36" t="n">
+        <v>0</v>
+      </c>
+      <c r="N36" t="inlineStr">
         <is>
           <t>m222615@dac.unicamp.br</t>
         </is>
@@ -2067,7 +2175,8 @@
       <c r="L37" t="n">
         <v>0</v>
       </c>
-      <c r="M37" t="inlineStr">
+      <c r="M37" t="inlineStr"/>
+      <c r="N37" t="inlineStr">
         <is>
           <t>s186966@dac.unicamp.br</t>
         </is>
@@ -2114,7 +2223,10 @@
       <c r="L38" t="n">
         <v>5</v>
       </c>
-      <c r="M38" t="inlineStr">
+      <c r="M38" t="n">
+        <v>0</v>
+      </c>
+      <c r="N38" t="inlineStr">
         <is>
           <t>s244321@dac.unicamp.br</t>
         </is>
@@ -2161,7 +2273,10 @@
       <c r="L39" t="n">
         <v>7</v>
       </c>
-      <c r="M39" t="inlineStr">
+      <c r="M39" t="n">
+        <v>0</v>
+      </c>
+      <c r="N39" t="inlineStr">
         <is>
           <t>s244379@dac.unicamp.br</t>
         </is>
@@ -2206,7 +2321,10 @@
       <c r="L40" t="n">
         <v>10</v>
       </c>
-      <c r="M40" t="inlineStr">
+      <c r="M40" t="n">
+        <v>81.72</v>
+      </c>
+      <c r="N40" t="inlineStr">
         <is>
           <t>t187323@dac.unicamp.br</t>
         </is>
@@ -2253,7 +2371,10 @@
       <c r="L41" t="n">
         <v>0</v>
       </c>
-      <c r="M41" t="inlineStr">
+      <c r="M41" t="n">
+        <v>0</v>
+      </c>
+      <c r="N41" t="inlineStr">
         <is>
           <t>t206194@dac.unicamp.br</t>
         </is>
@@ -2288,7 +2409,8 @@
       <c r="L42" t="n">
         <v>10</v>
       </c>
-      <c r="M42" t="inlineStr">
+      <c r="M42" t="inlineStr"/>
+      <c r="N42" t="inlineStr">
         <is>
           <t>v245212@dac.unicamp.br</t>
         </is>
@@ -2335,7 +2457,10 @@
       <c r="L43" t="n">
         <v>7</v>
       </c>
-      <c r="M43" t="inlineStr">
+      <c r="M43" t="n">
+        <v>0</v>
+      </c>
+      <c r="N43" t="inlineStr">
         <is>
           <t>v206883@dac.unicamp.br</t>
         </is>
@@ -2382,7 +2507,10 @@
       <c r="L44" t="n">
         <v>7</v>
       </c>
-      <c r="M44" t="inlineStr">
+      <c r="M44" t="n">
+        <v>10.75</v>
+      </c>
+      <c r="N44" t="inlineStr">
         <is>
           <t>v245459@dac.unicamp.br</t>
         </is>

</xml_diff>